<commit_message>
Se actualizaron varios archivos
Se actualizó checklist en el archivo Login-Pantallas.xlsx
Se eliminó el archivo registration.js y se unificó su código en el archivo index.js
Se creó el archivo validations.js que contiene el código para validación de campos input de los archivos registration.html y registration-en-html
</commit_message>
<xml_diff>
--- a/docs/Login-Pantallas.xlsx
+++ b/docs/Login-Pantallas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Desarrollo Web\Proyectos\Login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingja\Documents\GitHub\firebase-login\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFAE797-6485-456A-9C13-71C63759C8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B71C5B-7734-48FC-A1ED-E7119BEB0206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{A13D0670-B727-4968-91EA-75B449ECB28E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="6" xr2:uid="{A13D0670-B727-4968-91EA-75B449ECB28E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pantalla Inicio de sesión" sheetId="1" r:id="rId1"/>
@@ -323,11 +323,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2055,23 +2055,23 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.90625" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" customWidth="1"/>
-    <col min="11" max="11" width="68.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2080,7 +2080,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2091,7 +2091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2100,7 +2100,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2109,7 +2109,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -2120,7 +2120,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2129,7 +2129,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -2142,7 +2142,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2151,7 +2151,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -2164,7 +2164,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2173,7 +2173,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="s">
@@ -2186,7 +2186,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2195,7 +2195,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10" t="s">
@@ -2206,7 +2206,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2215,7 +2215,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2224,7 +2224,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2233,7 +2233,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2255,21 +2255,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.90625" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
-    <col min="8" max="8" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2278,7 +2278,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2289,7 +2289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2298,7 +2298,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2310,7 +2310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -2324,7 +2324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2336,7 +2336,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -2349,7 +2349,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2358,7 +2358,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -2371,7 +2371,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2380,7 +2380,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="s">
@@ -2393,7 +2393,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2402,7 +2402,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10" t="s">
@@ -2413,7 +2413,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2422,7 +2422,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2431,7 +2431,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2440,7 +2440,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2464,25 +2464,25 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="12"/>
@@ -2491,21 +2491,21 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="12"/>
       <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -2514,14 +2514,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -2530,14 +2530,14 @@
       <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -2546,14 +2546,14 @@
       <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="s">
@@ -2562,14 +2562,14 @@
       <c r="D11" s="6"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10" t="s">
@@ -2578,14 +2578,14 @@
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -2594,14 +2594,14 @@
       <c r="D15" s="9"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="2" t="s">
@@ -2610,14 +2610,14 @@
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="3" t="s">
@@ -2626,105 +2626,105 @@
       <c r="D19" s="9"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2746,14 +2746,14 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2762,7 +2762,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2773,7 +2773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2782,7 +2782,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2791,7 +2791,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -2802,7 +2802,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2811,7 +2811,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -2824,7 +2824,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2833,7 +2833,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -2846,7 +2846,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2855,7 +2855,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -2868,7 +2868,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2877,7 +2877,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11" t="s">
@@ -2888,7 +2888,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2897,7 +2897,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2906,7 +2906,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2915,7 +2915,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2938,14 +2938,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2954,7 +2954,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2965,7 +2965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2974,7 +2974,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2983,7 +2983,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -2994,7 +2994,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -3003,7 +3003,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -3016,7 +3016,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3025,7 +3025,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -3038,7 +3038,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -3047,7 +3047,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -3060,7 +3060,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3069,7 +3069,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11" t="s">
@@ -3080,7 +3080,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3089,7 +3089,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -3098,7 +3098,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -3107,7 +3107,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3130,25 +3130,25 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="12"/>
@@ -3157,21 +3157,21 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="12"/>
       <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -3180,14 +3180,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
@@ -3196,14 +3196,14 @@
       <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -3212,14 +3212,14 @@
       <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="13"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -3228,14 +3228,14 @@
       <c r="D11" s="6"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11" t="s">
@@ -3244,14 +3244,14 @@
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -3260,14 +3260,14 @@
       <c r="D15" s="9"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="2" t="s">
@@ -3276,14 +3276,14 @@
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="3" t="s">
@@ -3292,105 +3292,105 @@
       <c r="D19" s="9"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3408,28 +3408,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B5B290-E1FD-4948-9982-FFC8069989AF}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -3440,85 +3442,85 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -3528,8 +3530,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="s">
@@ -3539,8 +3541,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C14" t="s">
@@ -3550,8 +3552,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
@@ -3561,8 +3563,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
@@ -3572,8 +3574,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="15" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
@@ -3583,8 +3585,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="15" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
@@ -3594,8 +3596,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
@@ -3605,8 +3607,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
@@ -3616,8 +3618,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="15" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">

</xml_diff>